<commit_message>
Modulo FRONT END Completo
</commit_message>
<xml_diff>
--- a/resources/recaudacion20201.xlsx
+++ b/resources/recaudacion20201.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>sec</t>
   </si>
@@ -72,10 +72,10 @@
     <t>CEI- SubidoVie10_02</t>
   </si>
   <si>
-    <t>CEI- SubidoVie10_03</t>
-  </si>
-  <si>
-    <t>CEI- SubidoVie10_04</t>
+    <t>CEI- SubidoVie10_11</t>
+  </si>
+  <si>
+    <t>CEI- SubidoVie10_12</t>
   </si>
 </sst>
 </file>
@@ -559,8 +559,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,190 +947,519 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1981</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1">
+        <v>1754</v>
+      </c>
+      <c r="B2" s="1">
         <v>39323</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>87654321</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>87654325</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
         <v>110</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>20200107</v>
-      </c>
-      <c r="J2">
-        <v>122113</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>74</v>
-      </c>
-      <c r="M2">
-        <v>2186</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>20191103</v>
+      </c>
+      <c r="J2" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>401</v>
+      </c>
+      <c r="M2" s="1">
+        <v>71</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2655</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1">
+        <v>1755</v>
+      </c>
+      <c r="B3" s="1">
         <v>39323</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>87654320</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>87654325</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
         <v>110</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>20200109</v>
-      </c>
-      <c r="J3">
-        <v>122113</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>74</v>
-      </c>
-      <c r="M3">
-        <v>2186</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>20191203</v>
+      </c>
+      <c r="J3" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>401</v>
+      </c>
+      <c r="M3" s="1">
+        <v>71</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3719</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1">
+        <v>1756</v>
+      </c>
+      <c r="B4" s="1">
         <v>39323</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>87654319</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>87654323</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>110</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>20200104</v>
-      </c>
-      <c r="J4">
-        <v>83224</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>24</v>
-      </c>
-      <c r="M4">
-        <v>340</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>20191203</v>
+      </c>
+      <c r="J4" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>401</v>
+      </c>
+      <c r="M4" s="1">
+        <v>71</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
+        <v>1757</v>
+      </c>
+      <c r="B5" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>87654325</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>110</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>20200103</v>
+      </c>
+      <c r="J5" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>401</v>
+      </c>
+      <c r="M5" s="1">
+        <v>71</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1758</v>
+      </c>
+      <c r="B6" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>87654323</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>110</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>20200103</v>
+      </c>
+      <c r="J6" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>401</v>
+      </c>
+      <c r="M6" s="1">
+        <v>71</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1759</v>
+      </c>
+      <c r="B7" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>87654321</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>110</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1">
+        <v>20200103</v>
+      </c>
+      <c r="J7" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>401</v>
+      </c>
+      <c r="M7" s="1">
+        <v>71</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1760</v>
+      </c>
+      <c r="B8" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>87654324</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>110</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>20200103</v>
+      </c>
+      <c r="J8" s="1">
+        <v>84043</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>401</v>
+      </c>
+      <c r="M8" s="1">
+        <v>71</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B9" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>87654325</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>110</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>20200207</v>
+      </c>
+      <c r="J9" s="1">
+        <v>122113</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>74</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2186</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2655</v>
+      </c>
+      <c r="B10" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>87654323</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>110</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>20200209</v>
+      </c>
+      <c r="J10" s="1">
+        <v>122113</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>74</v>
+      </c>
+      <c r="M10" s="1">
+        <v>2186</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3719</v>
+      </c>
+      <c r="B11" s="1">
+        <v>39323</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>87654321</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>110</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>20200204</v>
+      </c>
+      <c r="J11" s="1">
+        <v>83224</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>24</v>
+      </c>
+      <c r="M11" s="1">
+        <v>340</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>4338</v>
       </c>
-      <c r="B5">
+      <c r="B12" s="1">
         <v>39323</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>87654318</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>87654324</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <v>110</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>20200103</v>
-      </c>
-      <c r="J5">
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>20200203</v>
+      </c>
+      <c r="J12" s="1">
         <v>84043</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>401</v>
       </c>
-      <c r="M5">
+      <c r="M12" s="1">
         <v>71</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>